<commit_message>
feat: add OpenXLSX demo
</commit_message>
<xml_diff>
--- a/inp/example.xlsx
+++ b/inp/example.xlsx
@@ -51,8 +51,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -360,13 +361,13 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>2</v>
       </c>
       <c r="B1">

</xml_diff>